<commit_message>
Add Delay:After svery step; Wait for presence of Web Element Corrected
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/FASB.xlsx
+++ b/src/main/resources/objectLocator/FASB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\objectLocator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCC855B-D8BA-4947-AED6-127F0526493D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA626E1-7E30-4CD6-9DEC-D08987F76B69}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FISchedule" sheetId="44" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="587">
   <si>
     <t>panelExportWidgetHeader</t>
   </si>
@@ -1774,9 +1774,6 @@
     <t>testamt.com</t>
   </si>
   <si>
-    <t>treeFASBMgr</t>
-  </si>
-  <si>
     <t>testamt.com/Accounts/FASBIASB/Index</t>
   </si>
   <si>
@@ -1796,6 +1793,12 @@
   </si>
   <si>
     <t>/Accounts/FASBIASB*FASB/IASB Revisions</t>
+  </si>
+  <si>
+    <t>//*[@class="k-widget k-treeview"]</t>
+  </si>
+  <si>
+    <t>//*[@id="treeFASBMgr"]</t>
   </si>
 </sst>
 </file>
@@ -3506,7 +3509,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3840,8 +3843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3961,7 +3964,7 @@
       </c>
       <c r="C8" s="23"/>
       <c r="E8" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3973,10 +3976,10 @@
       </c>
       <c r="C9" s="14"/>
       <c r="D9" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="E9" s="47" t="s">
-        <v>578</v>
+        <v>585</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3988,10 +3991,10 @@
       </c>
       <c r="C10" s="14"/>
       <c r="D10" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="E10" t="s">
-        <v>578</v>
+        <v>586</v>
       </c>
     </row>
   </sheetData>
@@ -4019,7 +4022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
@@ -4060,7 +4063,7 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="24" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E2"/>
     </row>
@@ -4075,7 +4078,7 @@
         <v>511</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E3" s="24" t="s">
         <v>571</v>
@@ -4134,7 +4137,7 @@
         <v>511</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E8" s="24" t="s">
         <v>571</v>
@@ -4151,7 +4154,7 @@
         <v>511</v>
       </c>
       <c r="D9" s="47" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E9" s="24" t="s">
         <v>571</v>
@@ -4223,7 +4226,7 @@
         <v>107</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E15" s="24" t="s">
         <v>571</v>
@@ -4240,7 +4243,7 @@
         <v>99</v>
       </c>
       <c r="D16" s="47" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E16" s="24" t="s">
         <v>571</v>

</xml_diff>